<commit_message>
Add new sample instances and update Profile Highlights and Guidance page
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-assistance-required.xlsx
+++ b/build/output/StructureDefinition-assistance-required.xlsx
@@ -384,42 +384,42 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="19.00390625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.1328125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="7.6796875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="19.59375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="12.65625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="8.95703125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="6.7734375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="4.9453125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="5.4296875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="16.2734375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.2578125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="14.44140625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="36.40625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="37.171875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="13.52734375" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="15.265625" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="15.7109375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="18.9140625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="17.07421875" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="17.7265625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="17.16796875" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="17.65625" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="19.03125" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="18.85546875" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="21.5703125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="19.625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="6.34765625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="22.71484375" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="42.03125" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="17.2109375" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="14.4140625" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="18.18359375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="10.55078125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="11.03515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="13.87109375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="36" max="36" width="22.671875" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="24.9765625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Prior level of function
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-assistance-required.xlsx
+++ b/build/output/StructureDefinition-assistance-required.xlsx
@@ -384,42 +384,42 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="19.59375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.65625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.95703125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="6.7734375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.9453125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="5.4296875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="16.2734375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="13.2578125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="14.44140625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="19.00390625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.1328125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="7.6796875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="37.171875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="36.40625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="15.265625" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="13.52734375" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="17.16796875" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="17.65625" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="19.03125" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="18.85546875" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="21.5703125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="19.625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="6.34765625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="22.71484375" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="42.03125" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="17.2109375" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="14.4140625" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="18.18359375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="10.55078125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="11.03515625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="13.87109375" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="15.7109375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="18.9140625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="17.07421875" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="17.7265625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="36" max="36" width="24.9765625" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="22.671875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Update PriorLevelOfFunction, IG web pages, and examples
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-assistance-required.xlsx
+++ b/build/output/StructureDefinition-assistance-required.xlsx
@@ -384,42 +384,42 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="19.00390625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.1328125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="7.6796875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="19.59375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="12.65625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="8.95703125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="6.7734375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="4.9453125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="5.4296875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="16.2734375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.2578125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="14.44140625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="36.40625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="37.171875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="13.52734375" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="15.265625" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="15.7109375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="18.9140625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="17.07421875" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="17.7265625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="17.16796875" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="17.65625" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="19.03125" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="18.85546875" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="21.5703125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="19.625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="6.34765625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="22.71484375" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="42.03125" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="17.2109375" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="14.4140625" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="18.18359375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="10.55078125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="11.03515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="13.87109375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="36" max="36" width="22.671875" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="24.9765625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
feedback from marc H.
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-assistance-required.xlsx
+++ b/build/output/StructureDefinition-assistance-required.xlsx
@@ -384,42 +384,42 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="19.59375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.65625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.95703125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="6.7734375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.9453125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="5.4296875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="16.2734375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="13.2578125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="14.44140625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="19.00390625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.1328125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="7.6796875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="37.171875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="36.40625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="15.265625" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="13.52734375" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="17.16796875" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="17.65625" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="19.03125" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="18.85546875" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="21.5703125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="19.625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="6.34765625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="22.71484375" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="42.03125" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="17.2109375" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="14.4140625" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="18.18359375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="10.55078125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="11.03515625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="13.87109375" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="15.7109375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="18.9140625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="17.07421875" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="17.7265625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="36" max="36" width="24.9765625" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="22.671875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Use new template hl7.fhir.template and fix sample data related QA errors
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-assistance-required.xlsx
+++ b/build/output/StructureDefinition-assistance-required.xlsx
@@ -206,7 +206,7 @@
     <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition SHALL be a URI for the Structure Definition defining the extension.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/functional-status-ig/StructureDefinition/assistance-required</t>
+    <t>http://hl7.org/fhir/us/pacio-fs/StructureDefinition/assistance-required</t>
   </si>
   <si>
     <t>N/A</t>
@@ -384,42 +384,42 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="19.00390625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.1328125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="7.6796875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="19.59375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="12.65625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="8.95703125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="6.7734375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="4.9453125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="5.4296875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="16.2734375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.2578125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="14.44140625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="36.40625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="37.171875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="13.52734375" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="15.265625" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="15.7109375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="18.9140625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="17.07421875" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="17.7265625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="17.16796875" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="17.65625" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="19.03125" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="18.85546875" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="21.5703125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="19.625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="6.34765625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="22.71484375" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="42.03125" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="17.2109375" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="14.4140625" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="18.18359375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="10.55078125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="11.03515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="13.87109375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="36" max="36" width="22.671875" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="24.9765625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
added CMS assessment label
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-assistance-required.xlsx
+++ b/build/output/StructureDefinition-assistance-required.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="69">
   <si>
     <t>Path</t>
   </si>
@@ -137,7 +137,7 @@
     <t>*</t>
   </si>
   <si>
-    <t>An Extension</t>
+    <t>Associated functional status used for display purposes.</t>
   </si>
   <si>
     <t xml:space="preserve">ele-1
@@ -175,6 +175,9 @@
   <si>
     <t xml:space="preserve">Extension
 </t>
+  </si>
+  <si>
+    <t>An Extension</t>
   </si>
   <si>
     <t xml:space="preserve">value:url}
@@ -763,7 +766,7 @@
         <v>36</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -802,19 +805,19 @@
         <v>37</v>
       </c>
       <c r="AA4" t="s" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AB4" t="s" s="2">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AC4" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AD4" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AE4" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AF4" t="s" s="2">
         <v>38</v>
@@ -834,7 +837,7 @@
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
@@ -857,16 +860,16 @@
         <v>37</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="M5" t="s" s="2">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" t="s" s="2">
@@ -874,7 +877,7 @@
       </c>
       <c r="P5" s="2"/>
       <c r="Q5" t="s" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R5" t="s" s="2">
         <v>37</v>
@@ -916,7 +919,7 @@
         <v>37</v>
       </c>
       <c r="AE5" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AF5" t="s" s="2">
         <v>44</v>
@@ -931,12 +934,12 @@
         <v>37</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
@@ -959,13 +962,13 @@
         <v>37</v>
       </c>
       <c r="J6" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -1016,7 +1019,7 @@
         <v>37</v>
       </c>
       <c r="AE6" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AF6" t="s" s="2">
         <v>38</v>
@@ -1028,10 +1031,10 @@
         <v>37</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AJ6" t="s" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add changes for block vote items
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-assistance-required.xlsx
+++ b/build/output/StructureDefinition-assistance-required.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="69">
   <si>
     <t>Path</t>
   </si>
@@ -137,7 +137,7 @@
     <t>*</t>
   </si>
   <si>
-    <t>An Extension</t>
+    <t>Associated functional status used for display purposes.</t>
   </si>
   <si>
     <t xml:space="preserve">ele-1
@@ -175,6 +175,9 @@
   <si>
     <t xml:space="preserve">Extension
 </t>
+  </si>
+  <si>
+    <t>An Extension</t>
   </si>
   <si>
     <t xml:space="preserve">value:url}
@@ -763,7 +766,7 @@
         <v>36</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -802,19 +805,19 @@
         <v>37</v>
       </c>
       <c r="AA4" t="s" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AB4" t="s" s="2">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AC4" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AD4" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AE4" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AF4" t="s" s="2">
         <v>38</v>
@@ -834,7 +837,7 @@
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
@@ -857,16 +860,16 @@
         <v>37</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="M5" t="s" s="2">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" t="s" s="2">
@@ -874,7 +877,7 @@
       </c>
       <c r="P5" s="2"/>
       <c r="Q5" t="s" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R5" t="s" s="2">
         <v>37</v>
@@ -916,7 +919,7 @@
         <v>37</v>
       </c>
       <c r="AE5" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AF5" t="s" s="2">
         <v>44</v>
@@ -931,12 +934,12 @@
         <v>37</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
@@ -959,13 +962,13 @@
         <v>37</v>
       </c>
       <c r="J6" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -1016,7 +1019,7 @@
         <v>37</v>
       </c>
       <c r="AE6" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AF6" t="s" s="2">
         <v>38</v>
@@ -1028,10 +1031,10 @@
         <v>37</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AJ6" t="s" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add changes for Block Votes 1 and 2 items
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-assistance-required.xlsx
+++ b/build/output/StructureDefinition-assistance-required.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="71">
   <si>
     <t>Path</t>
   </si>
@@ -137,7 +137,7 @@
     <t>*</t>
   </si>
   <si>
-    <t>Associated functional status used for display purposes.</t>
+    <t>Associated with prior level of function to provide a high-level indication of assistance required for the person’s baseline ability (physical function immediately preceding the current admission, illness, or exacerbation for a patient) to answer functional related clinical questions. The CMS Assessment answer list LL4309-2 provides possible values for this extension.</t>
   </si>
   <si>
     <t xml:space="preserve">ele-1
@@ -226,6 +226,12 @@
   </si>
   <si>
     <t>Value of extension - must be one of a constrained set of the data types (see [Extensibility](http://hl7.org/fhir/R4/extensibility.html) for a list).</t>
+  </si>
+  <si>
+    <t>extensible</t>
+  </si>
+  <si>
+    <t>http://loinc.org/vs/LL4309-2</t>
   </si>
   <si>
     <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
@@ -411,7 +417,7 @@
     <col min="22" max="22" width="19.03125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="18.85546875" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="21.5703125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="19.625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="26.40234375" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="6.34765625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="22.71484375" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="42.03125" customWidth="true" bestFit="true"/>
@@ -995,13 +1001,11 @@
         <v>37</v>
       </c>
       <c r="W6" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="X6" t="s" s="2">
-        <v>37</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="X6" s="2"/>
       <c r="Y6" t="s" s="2">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="Z6" t="s" s="2">
         <v>37</v>
@@ -1031,7 +1035,7 @@
         <v>37</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="AJ6" t="s" s="2">
         <v>63</v>

</xml_diff>